<commit_message>
editados los description para ponerles palabras clave
</commit_message>
<xml_diff>
--- a/Hoja de cálculo Proyecto1-Fase4-SEO.xlsx
+++ b/Hoja de cálculo Proyecto1-Fase4-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <r>
       <rPr>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">Blood bowl team manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood bowl</t>
   </si>
   <si>
     <t xml:space="preserve">Wikipedia Table of Contents</t>
@@ -643,7 +646,7 @@
   <dimension ref="A1:Z70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5078125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -774,7 +777,9 @@
       <c r="D4" s="10" t="n">
         <v>0.14</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9" t="n">
+        <v>29</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="11"/>
@@ -808,7 +813,9 @@
       <c r="D5" s="10" t="n">
         <v>0.06</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9" t="n">
+        <v>33</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="11"/>
@@ -833,10 +840,16 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="12"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>2900</v>
+      </c>
       <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="E6" s="13" t="n">
+        <v>31</v>
+      </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="11"/>
@@ -945,7 +958,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
@@ -1115,7 +1128,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="13"/>
@@ -1285,7 +1298,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
@@ -1455,7 +1468,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1625,7 +1638,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
@@ -1795,7 +1808,7 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -1965,7 +1978,7 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -2135,7 +2148,7 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>

</xml_diff>